<commit_message>
added slides in F13 on discrete simultaneous dist
</commit_message>
<xml_diff>
--- a/misc/DiskretSimultanfördelningKovarians.xlsx
+++ b/misc/DiskretSimultanfördelningKovarians.xlsx
@@ -494,11 +494,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="484503357"/>
-        <c:axId val="1748660856"/>
+        <c:axId val="616556659"/>
+        <c:axId val="243431230"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="484503357"/>
+        <c:axId val="616556659"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -550,10 +550,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1748660856"/>
+        <c:crossAx val="243431230"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1748660856"/>
+        <c:axId val="243431230"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -628,7 +628,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="484503357"/>
+        <c:crossAx val="616556659"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -714,11 +714,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1492593301"/>
-        <c:axId val="1041525936"/>
+        <c:axId val="916269430"/>
+        <c:axId val="1281372616"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1492593301"/>
+        <c:axId val="916269430"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -770,10 +770,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1041525936"/>
+        <c:crossAx val="1281372616"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1041525936"/>
+        <c:axId val="1281372616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -848,7 +848,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1492593301"/>
+        <c:crossAx val="916269430"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1241,11 +1241,11 @@
             </c:numLit>
           </c:bubbleSize>
         </c:ser>
-        <c:axId val="1766603449"/>
-        <c:axId val="1358739365"/>
+        <c:axId val="1532994061"/>
+        <c:axId val="1874232994"/>
       </c:bubbleChart>
       <c:valAx>
-        <c:axId val="1766603449"/>
+        <c:axId val="1532994061"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="3.0"/>
@@ -1321,10 +1321,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1358739365"/>
+        <c:crossAx val="1874232994"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1358739365"/>
+        <c:axId val="1874232994"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="3.0"/>
@@ -1400,7 +1400,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1766603449"/>
+        <c:crossAx val="1532994061"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2291,8 +2291,8 @@
       <c r="B24" s="16"/>
       <c r="C24" s="16"/>
       <c r="H24" s="20">
-        <f>(C8-$G$18)^2*C12 + (D8-$G$18)^2*D12 + (D8-$G$18)^2*D12</f>
-        <v>0.293584</v>
+        <f>(C8-$G$18)^2*C12 + (D8-$G$18)^2*D12 + (E8-$G$18)^2*E12</f>
+        <v>0.5876</v>
       </c>
       <c r="J24" s="22" t="s">
         <v>14</v>
@@ -2300,7 +2300,7 @@
       <c r="K24" s="23"/>
       <c r="L24" s="20">
         <f>SQRT(H24)</f>
-        <v>0.5418339229</v>
+        <v>0.7665507159</v>
       </c>
     </row>
     <row r="26">
@@ -2326,7 +2326,7 @@
       <c r="E31" s="27"/>
       <c r="I31" s="20">
         <f>J26/(L21*L24)</f>
-        <v>0.7652939039</v>
+        <v>0.5409455494</v>
       </c>
     </row>
     <row r="34">

</xml_diff>